<commit_message>
added rating and website
</commit_message>
<xml_diff>
--- a/Indianapolis-Day-Plan.xlsx
+++ b/Indianapolis-Day-Plan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Time</t>
   </si>
@@ -19,6 +19,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Rating</t>
+  </si>
+  <si>
     <t>Address</t>
   </si>
   <si>
@@ -28,6 +31,9 @@
     <t>Duration</t>
   </si>
   <si>
+    <t>Website</t>
+  </si>
+  <si>
     <t>Indianapolis Zoo</t>
   </si>
   <si>
@@ -40,6 +46,9 @@
     <t>3 hours</t>
   </si>
   <si>
+    <t>http://www.indianapoliszoo.com/</t>
+  </si>
+  <si>
     <t>Garfield Park Conservatory</t>
   </si>
   <si>
@@ -52,6 +61,9 @@
     <t>2 hours</t>
   </si>
   <si>
+    <t>https://www.garfieldgardensconservatory.org/</t>
+  </si>
+  <si>
     <t>Indiana State Museum</t>
   </si>
   <si>
@@ -61,12 +73,18 @@
     <t>museum</t>
   </si>
   <si>
+    <t>http://www.indianamuseum.org/</t>
+  </si>
+  <si>
     <t>The Escape Room Indianapolis</t>
   </si>
   <si>
     <t>200 S Meridian St STE 220, Indianapolis</t>
   </si>
   <si>
+    <t>https://escaperoomindy.com/</t>
+  </si>
+  <si>
     <t>The Old Spaghetti Factory</t>
   </si>
   <si>
@@ -74,6 +92,9 @@
   </si>
   <si>
     <t>dinner</t>
+  </si>
+  <si>
+    <t>https://www.osf.com/location/indianapolis-in/</t>
   </si>
 </sst>
 </file>
@@ -83,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm am/pm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -99,6 +120,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -125,20 +150,26 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -359,8 +390,10 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="11.75"/>
     <col customWidth="1" min="2" max="2" width="24.13"/>
-    <col customWidth="1" min="3" max="3" width="31.75"/>
-    <col customWidth="1" min="4" max="4" width="13.38"/>
+    <col customWidth="1" min="3" max="3" width="6.13"/>
+    <col customWidth="1" min="4" max="4" width="31.75"/>
+    <col customWidth="1" min="5" max="5" width="13.38"/>
+    <col customWidth="1" min="7" max="7" width="34.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -370,7 +403,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -379,93 +412,136 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>0.375</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4.5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>0.5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>0.5833333333333334</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4.6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>0.7083333333333334</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4.8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="4">
         <v>0.7916666666666666</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId2" ref="G3"/>
+    <hyperlink r:id="rId3" ref="G4"/>
+    <hyperlink r:id="rId4" ref="G5"/>
+    <hyperlink r:id="rId5" ref="G6"/>
+  </hyperlinks>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>